<commit_message>
K and 1/n uncertainty analysis
Analyse isotherm parameters
</commit_message>
<xml_diff>
--- a/1USEPA_PSDM/5PSDM_EditMathieu/Example_TCE.xlsx
+++ b/1USEPA_PSDM/5PSDM_EditMathieu/Example_TCE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JBurkhar\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\Git\PSDM\PSDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Activated-Carbon-Modelling\1USEPA_PSDM\5PSDM_EditMathieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{41008640-FEA6-4E03-9782-ECE2DD9879EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B504F409-C663-4716-84E1-AD7051C94A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,15 +282,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +355,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,18 +617,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -639,7 +636,7 @@
         <v>131.38999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -647,7 +644,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -655,7 +652,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -663,19 +660,19 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>9830</v>
       </c>
     </row>
@@ -688,18 +685,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB297697-1B90-46DD-B82E-FCE20BA48421}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -707,15 +704,15 @@
         <v>5026.04</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -723,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -731,7 +728,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -752,160 +749,160 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>5.1299999999999998E-2</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0.80300000000000005</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0.62</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2.7650000000000001</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>20000</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>566.96600000000001</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -922,15 +919,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -944,7 +941,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -954,11 +951,11 @@
       <c r="C2">
         <v>50000</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -972,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -986,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1013,15 +1010,15 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1045,11 +1042,11 @@
       <c r="C2">
         <v>3000</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1059,11 +1056,11 @@
       <c r="C3">
         <v>2000</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1073,11 +1070,11 @@
       <c r="C4">
         <v>4000</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1132,62 +1129,62 @@
       <selection activeCell="A3" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="148" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="148" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A2" s="8">
+    <row r="2" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A3" s="8">
+    <row r="3" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="157.5" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
+    <row r="4" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="94.5" x14ac:dyDescent="0.5">
-      <c r="A6" s="8">
+    <row r="6" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A7" s="8">
+    <row r="7" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A9" s="8">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1200,19 +1197,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0262868-F1D2-4471-83DF-330B743CAC3B}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1236,11 +1233,11 @@
       <c r="C2">
         <v>1500</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1250,11 +1247,11 @@
       <c r="C3">
         <v>1250</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1264,11 +1261,11 @@
       <c r="C4">
         <v>1000</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1296,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1324,7 +1321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1394,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1408,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1464,7 +1461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1492,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1506,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1520,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1534,7 +1531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1576,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1590,7 +1587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1610,6 +1607,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3E377063FFE5489A04E78E6AF321F7" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d56b0910c09b2f28088e837fc8a4b1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns4="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns6="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xmlns:ns7="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c38d2d5698dbedce593845e142ad0a0f" ns1:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2066,62 +2118,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2142,41 +2176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>